<commit_message>
School Dist data cleaning
</commit_message>
<xml_diff>
--- a/Data/2020alarms.org_top500schooldist.xlsx
+++ b/Data/2020alarms.org_top500schooldist.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danbishop/Desktop/Passion Projects/HomeSlice/HomeSlice/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC12752-AAD2-A24B-82F2-189E611EF065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCC178F-F6CE-8641-A1F3-EF7775C7FAC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="960" windowWidth="27360" windowHeight="16540" xr2:uid="{69217F67-C01E-1F4A-BFEF-6A6F1764DCD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$501</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -761,9 +764,6 @@
     <t>Colorado</t>
   </si>
   <si>
-    <t>CHEYENNE MOUNTAIN SCHOOL DISTRICT NO. 12, IN THE COUNTY OF E</t>
-  </si>
-  <si>
     <t>TROY SCHOOL DISTRICT</t>
   </si>
   <si>
@@ -1100,9 +1100,6 @@
     <t>COLD SPRING HARBOR CENTRAL SCHOOL DISTRICT</t>
   </si>
   <si>
-    <t>BROWNSBURG COMMUNITY SCH CORP</t>
-  </si>
-  <si>
     <t>PLEASANT VALLEY COMM SCHOOL DISTRICT</t>
   </si>
   <si>
@@ -1223,9 +1220,6 @@
     <t>CARMEL UNIFIED</t>
   </si>
   <si>
-    <t>SOUTHEAST DUBOIS CO SCH CORP</t>
-  </si>
-  <si>
     <t>HAMPDEN-WILBRAHAM</t>
   </si>
   <si>
@@ -1247,9 +1241,6 @@
     <t>ARGYLE ISD</t>
   </si>
   <si>
-    <t>ACADEMY, SCHOOL DISTRICT NO. 20, IN THE COUNTY OF EL PASO AN</t>
-  </si>
-  <si>
     <t>GERMANTOWN SCHOOL DISTRICT</t>
   </si>
   <si>
@@ -1277,9 +1268,6 @@
     <t>MONTCLAIR PUBLIC SCHOOLS</t>
   </si>
   <si>
-    <t>LITTLETON, SCHOOL DISTRICT NO. 6, IN THE COUNTY OF ARAPAHOE</t>
-  </si>
-  <si>
     <t>DUMONT BOARD OF EDUCATION</t>
   </si>
   <si>
@@ -1334,9 +1322,6 @@
     <t>DE PERE SCHOOL DISTRICT</t>
   </si>
   <si>
-    <t>LEWIS-PALMER CONSOLIDATED, SCHOOL DISTRICT NO. 38, IN THE CO</t>
-  </si>
-  <si>
     <t>FRANKLIN PUBLIC SCHOOL DISTRICT</t>
   </si>
   <si>
@@ -1361,9 +1346,6 @@
     <t>CALDWELL-WEST CALDWELL PUBLIC SCHOOLS</t>
   </si>
   <si>
-    <t>ST. MICHAEL-ALBERTVILLE SCHOOL DIST</t>
-  </si>
-  <si>
     <t>WADSWORTH CITY</t>
   </si>
   <si>
@@ -1475,9 +1457,6 @@
     <t>Virginia</t>
   </si>
   <si>
-    <t>FALLS CHURCH CITY PBLC SCHS</t>
-  </si>
-  <si>
     <t>PORT ARANSAS ISD</t>
   </si>
   <si>
@@ -1541,9 +1520,6 @@
     <t>WAUWATOSA SCHOOL DISTRICT</t>
   </si>
   <si>
-    <t>STILLWATER AREA PUBLIC SCHOOL DIST.</t>
-  </si>
-  <si>
     <t>ASPEN SCHOOL DISTRICT</t>
   </si>
   <si>
@@ -1583,21 +1559,12 @@
     <t>AMHERST-PELHAM</t>
   </si>
   <si>
-    <t>ARLINGTON CO PBLC SCHS</t>
-  </si>
-  <si>
     <t>LAKE ZURICH CUSD 95</t>
   </si>
   <si>
-    <t>SOUTH WASHINGTON COUNTY SCHOOL DIST</t>
-  </si>
-  <si>
     <t>FOREST HILLS PUBLIC SCHOOLS</t>
   </si>
   <si>
-    <t>NORTH SPENCER COUNTY SCH CORP</t>
-  </si>
-  <si>
     <t>CATALINA FOOTHILLS UNIFIED DISTRICT</t>
   </si>
   <si>
@@ -1641,6 +1608,42 @@
   </si>
   <si>
     <t>BURNT HILLS-BALLSTON LAKE CENTRAL SCHOOL DISTRICT</t>
+  </si>
+  <si>
+    <t>CHEYENNE MOUNTAIN SCHOOL DISTRICT NO. 12</t>
+  </si>
+  <si>
+    <t>BROWNSBURG COMMUNITY</t>
+  </si>
+  <si>
+    <t>SOUTHEAST DUBOIS</t>
+  </si>
+  <si>
+    <t>ACADEMY, SCHOOL DISTRICT NO. 20</t>
+  </si>
+  <si>
+    <t>LITTLETON, SCHOOL DISTRICT NO. 6</t>
+  </si>
+  <si>
+    <t>LEWIS-PALMER CONSOLIDATED, SCHOOL DISTRICT NO. 38,</t>
+  </si>
+  <si>
+    <t>FALLS CHURCH CITY</t>
+  </si>
+  <si>
+    <t>STILLWATER AREA PUBLIC SCHOOL</t>
+  </si>
+  <si>
+    <t>ARLINGTON CO</t>
+  </si>
+  <si>
+    <t>NORTH SPENCER COUNTY</t>
+  </si>
+  <si>
+    <t>SOUTH WASHINGTON COUNTY SCHOOL</t>
+  </si>
+  <si>
+    <t>ST. MICHAEL-ALBERTVILLE SCHOOL</t>
   </si>
 </sst>
 </file>
@@ -1995,7 +1998,7 @@
   <dimension ref="A1:C501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4384,7 +4387,7 @@
         <v>241</v>
       </c>
       <c r="C217" t="s">
-        <v>242</v>
+        <v>524</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
@@ -4395,7 +4398,7 @@
         <v>154</v>
       </c>
       <c r="C218" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
@@ -4406,7 +4409,7 @@
         <v>6</v>
       </c>
       <c r="C219" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
@@ -4417,7 +4420,7 @@
         <v>36</v>
       </c>
       <c r="C220" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
@@ -4428,7 +4431,7 @@
         <v>6</v>
       </c>
       <c r="C221" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
@@ -4439,7 +4442,7 @@
         <v>198</v>
       </c>
       <c r="C222" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
@@ -4450,7 +4453,7 @@
         <v>177</v>
       </c>
       <c r="C223" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
@@ -4461,7 +4464,7 @@
         <v>11</v>
       </c>
       <c r="C224" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
@@ -4472,7 +4475,7 @@
         <v>36</v>
       </c>
       <c r="C225" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
@@ -4483,7 +4486,7 @@
         <v>241</v>
       </c>
       <c r="C226" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
@@ -4494,7 +4497,7 @@
         <v>154</v>
       </c>
       <c r="C227" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
@@ -4505,7 +4508,7 @@
         <v>154</v>
       </c>
       <c r="C228" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
@@ -4516,7 +4519,7 @@
         <v>29</v>
       </c>
       <c r="C229" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
@@ -4527,7 +4530,7 @@
         <v>29</v>
       </c>
       <c r="C230" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
@@ -4538,7 +4541,7 @@
         <v>29</v>
       </c>
       <c r="C231" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
@@ -4549,7 +4552,7 @@
         <v>36</v>
       </c>
       <c r="C232" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
@@ -4560,7 +4563,7 @@
         <v>44</v>
       </c>
       <c r="C233" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
@@ -4571,7 +4574,7 @@
         <v>6</v>
       </c>
       <c r="C234" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
@@ -4582,7 +4585,7 @@
         <v>29</v>
       </c>
       <c r="C235" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
@@ -4593,7 +4596,7 @@
         <v>198</v>
       </c>
       <c r="C236" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
@@ -4604,7 +4607,7 @@
         <v>132</v>
       </c>
       <c r="C237" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
@@ -4615,7 +4618,7 @@
         <v>90</v>
       </c>
       <c r="C238" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
@@ -4626,7 +4629,7 @@
         <v>36</v>
       </c>
       <c r="C239" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
@@ -4637,7 +4640,7 @@
         <v>36</v>
       </c>
       <c r="C240" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
@@ -4648,7 +4651,7 @@
         <v>44</v>
       </c>
       <c r="C241" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
@@ -4659,7 +4662,7 @@
         <v>198</v>
       </c>
       <c r="C242" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
@@ -4670,7 +4673,7 @@
         <v>44</v>
       </c>
       <c r="C243" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
@@ -4681,7 +4684,7 @@
         <v>241</v>
       </c>
       <c r="C244" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
@@ -4692,7 +4695,7 @@
         <v>90</v>
       </c>
       <c r="C245" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
@@ -4703,7 +4706,7 @@
         <v>11</v>
       </c>
       <c r="C246" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
@@ -4714,7 +4717,7 @@
         <v>6</v>
       </c>
       <c r="C247" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
@@ -4725,7 +4728,7 @@
         <v>3</v>
       </c>
       <c r="C248" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
@@ -4736,7 +4739,7 @@
         <v>29</v>
       </c>
       <c r="C249" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
@@ -4747,7 +4750,7 @@
         <v>198</v>
       </c>
       <c r="C250" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
@@ -4758,7 +4761,7 @@
         <v>61</v>
       </c>
       <c r="C251" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
@@ -4769,7 +4772,7 @@
         <v>6</v>
       </c>
       <c r="C252" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
@@ -4780,7 +4783,7 @@
         <v>29</v>
       </c>
       <c r="C253" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
@@ -4791,7 +4794,7 @@
         <v>54</v>
       </c>
       <c r="C254" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
@@ -4802,7 +4805,7 @@
         <v>44</v>
       </c>
       <c r="C255" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
@@ -4813,7 +4816,7 @@
         <v>29</v>
       </c>
       <c r="C256" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
@@ -4824,7 +4827,7 @@
         <v>6</v>
       </c>
       <c r="C257" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
@@ -4835,7 +4838,7 @@
         <v>18</v>
       </c>
       <c r="C258" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
@@ -4846,7 +4849,7 @@
         <v>44</v>
       </c>
       <c r="C259" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
@@ -4854,10 +4857,10 @@
         <v>259</v>
       </c>
       <c r="B260" t="s">
+        <v>284</v>
+      </c>
+      <c r="C260" t="s">
         <v>285</v>
-      </c>
-      <c r="C260" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
@@ -4868,7 +4871,7 @@
         <v>44</v>
       </c>
       <c r="C261" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
@@ -4879,7 +4882,7 @@
         <v>29</v>
       </c>
       <c r="C262" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
@@ -4890,7 +4893,7 @@
         <v>11</v>
       </c>
       <c r="C263" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
@@ -4901,7 +4904,7 @@
         <v>18</v>
       </c>
       <c r="C264" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
@@ -4912,7 +4915,7 @@
         <v>90</v>
       </c>
       <c r="C265" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
@@ -4923,7 +4926,7 @@
         <v>11</v>
       </c>
       <c r="C266" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
@@ -4934,7 +4937,7 @@
         <v>11</v>
       </c>
       <c r="C267" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
@@ -4945,7 +4948,7 @@
         <v>154</v>
       </c>
       <c r="C268" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
@@ -4956,7 +4959,7 @@
         <v>6</v>
       </c>
       <c r="C269" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
@@ -4967,7 +4970,7 @@
         <v>150</v>
       </c>
       <c r="C270" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
@@ -4978,7 +4981,7 @@
         <v>6</v>
       </c>
       <c r="C271" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
@@ -4989,7 +4992,7 @@
         <v>44</v>
       </c>
       <c r="C272" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
@@ -5000,7 +5003,7 @@
         <v>29</v>
       </c>
       <c r="C273" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
@@ -5011,7 +5014,7 @@
         <v>29</v>
       </c>
       <c r="C274" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
@@ -5022,7 +5025,7 @@
         <v>6</v>
       </c>
       <c r="C275" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
@@ -5033,7 +5036,7 @@
         <v>6</v>
       </c>
       <c r="C276" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
@@ -5044,7 +5047,7 @@
         <v>36</v>
       </c>
       <c r="C277" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
@@ -5055,7 +5058,7 @@
         <v>36</v>
       </c>
       <c r="C278" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
@@ -5066,7 +5069,7 @@
         <v>11</v>
       </c>
       <c r="C279" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
@@ -5077,7 +5080,7 @@
         <v>44</v>
       </c>
       <c r="C280" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
@@ -5088,7 +5091,7 @@
         <v>44</v>
       </c>
       <c r="C281" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
@@ -5099,7 +5102,7 @@
         <v>90</v>
       </c>
       <c r="C282" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
@@ -5110,7 +5113,7 @@
         <v>154</v>
       </c>
       <c r="C283" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
@@ -5121,7 +5124,7 @@
         <v>3</v>
       </c>
       <c r="C284" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
@@ -5132,7 +5135,7 @@
         <v>36</v>
       </c>
       <c r="C285" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
@@ -5143,7 +5146,7 @@
         <v>29</v>
       </c>
       <c r="C286" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
@@ -5154,7 +5157,7 @@
         <v>90</v>
       </c>
       <c r="C287" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
@@ -5165,7 +5168,7 @@
         <v>90</v>
       </c>
       <c r="C288" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
@@ -5173,10 +5176,10 @@
         <v>288</v>
       </c>
       <c r="B289" t="s">
+        <v>314</v>
+      </c>
+      <c r="C289" t="s">
         <v>315</v>
-      </c>
-      <c r="C289" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
@@ -5187,7 +5190,7 @@
         <v>61</v>
       </c>
       <c r="C290" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
@@ -5198,7 +5201,7 @@
         <v>68</v>
       </c>
       <c r="C291" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
@@ -5209,7 +5212,7 @@
         <v>6</v>
       </c>
       <c r="C292" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
@@ -5220,7 +5223,7 @@
         <v>29</v>
       </c>
       <c r="C293" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
@@ -5231,7 +5234,7 @@
         <v>11</v>
       </c>
       <c r="C294" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
@@ -5239,10 +5242,10 @@
         <v>294</v>
       </c>
       <c r="B295" t="s">
+        <v>321</v>
+      </c>
+      <c r="C295" t="s">
         <v>322</v>
-      </c>
-      <c r="C295" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
@@ -5253,7 +5256,7 @@
         <v>6</v>
       </c>
       <c r="C296" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
@@ -5264,7 +5267,7 @@
         <v>6</v>
       </c>
       <c r="C297" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
@@ -5275,7 +5278,7 @@
         <v>29</v>
       </c>
       <c r="C298" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
@@ -5286,7 +5289,7 @@
         <v>27</v>
       </c>
       <c r="C299" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
@@ -5297,7 +5300,7 @@
         <v>18</v>
       </c>
       <c r="C300" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
@@ -5305,10 +5308,10 @@
         <v>300</v>
       </c>
       <c r="B301" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C301" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
@@ -5319,7 +5322,7 @@
         <v>44</v>
       </c>
       <c r="C302" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
@@ -5330,7 +5333,7 @@
         <v>44</v>
       </c>
       <c r="C303" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
@@ -5341,7 +5344,7 @@
         <v>11</v>
       </c>
       <c r="C304" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
@@ -5352,7 +5355,7 @@
         <v>6</v>
       </c>
       <c r="C305" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
@@ -5363,7 +5366,7 @@
         <v>36</v>
       </c>
       <c r="C306" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
@@ -5374,7 +5377,7 @@
         <v>29</v>
       </c>
       <c r="C307" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
@@ -5385,7 +5388,7 @@
         <v>44</v>
       </c>
       <c r="C308" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
@@ -5396,7 +5399,7 @@
         <v>29</v>
       </c>
       <c r="C309" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.2">
@@ -5404,10 +5407,10 @@
         <v>309</v>
       </c>
       <c r="B310" t="s">
+        <v>337</v>
+      </c>
+      <c r="C310" t="s">
         <v>338</v>
-      </c>
-      <c r="C310" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.2">
@@ -5418,7 +5421,7 @@
         <v>6</v>
       </c>
       <c r="C311" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.2">
@@ -5426,10 +5429,10 @@
         <v>311</v>
       </c>
       <c r="B312" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C312" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
@@ -5440,7 +5443,7 @@
         <v>36</v>
       </c>
       <c r="C313" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
@@ -5451,7 +5454,7 @@
         <v>44</v>
       </c>
       <c r="C314" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
@@ -5462,7 +5465,7 @@
         <v>6</v>
       </c>
       <c r="C315" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
@@ -5473,7 +5476,7 @@
         <v>154</v>
       </c>
       <c r="C316" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
@@ -5484,7 +5487,7 @@
         <v>61</v>
       </c>
       <c r="C317" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
@@ -5495,7 +5498,7 @@
         <v>11</v>
       </c>
       <c r="C318" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
@@ -5506,7 +5509,7 @@
         <v>11</v>
       </c>
       <c r="C319" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
@@ -5517,7 +5520,7 @@
         <v>198</v>
       </c>
       <c r="C320" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
@@ -5528,7 +5531,7 @@
         <v>44</v>
       </c>
       <c r="C321" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
@@ -5539,7 +5542,7 @@
         <v>44</v>
       </c>
       <c r="C322" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
@@ -5550,7 +5553,7 @@
         <v>44</v>
       </c>
       <c r="C323" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
@@ -5561,7 +5564,7 @@
         <v>11</v>
       </c>
       <c r="C324" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
@@ -5572,7 +5575,7 @@
         <v>44</v>
       </c>
       <c r="C325" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
@@ -5583,7 +5586,7 @@
         <v>59</v>
       </c>
       <c r="C326" t="s">
-        <v>355</v>
+        <v>525</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
@@ -5591,10 +5594,10 @@
         <v>326</v>
       </c>
       <c r="B327" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C327" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
@@ -5602,10 +5605,10 @@
         <v>327</v>
       </c>
       <c r="B328" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C328" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
@@ -5616,7 +5619,7 @@
         <v>36</v>
       </c>
       <c r="C329" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
@@ -5627,7 +5630,7 @@
         <v>6</v>
       </c>
       <c r="C330" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
@@ -5638,7 +5641,7 @@
         <v>68</v>
       </c>
       <c r="C331" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
@@ -5649,7 +5652,7 @@
         <v>36</v>
       </c>
       <c r="C332" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
@@ -5660,7 +5663,7 @@
         <v>11</v>
       </c>
       <c r="C333" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
@@ -5671,7 +5674,7 @@
         <v>36</v>
       </c>
       <c r="C334" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
@@ -5682,7 +5685,7 @@
         <v>27</v>
       </c>
       <c r="C335" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
@@ -5693,7 +5696,7 @@
         <v>61</v>
       </c>
       <c r="C336" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
@@ -5704,7 +5707,7 @@
         <v>150</v>
       </c>
       <c r="C337" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
@@ -5712,10 +5715,10 @@
         <v>337</v>
       </c>
       <c r="B338" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C338" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.2">
@@ -5723,10 +5726,10 @@
         <v>338</v>
       </c>
       <c r="B339" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C339" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.2">
@@ -5737,7 +5740,7 @@
         <v>177</v>
       </c>
       <c r="C340" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
@@ -5756,10 +5759,10 @@
         <v>341</v>
       </c>
       <c r="B342" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C342" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.2">
@@ -5770,7 +5773,7 @@
         <v>3</v>
       </c>
       <c r="C343" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.2">
@@ -5781,7 +5784,7 @@
         <v>36</v>
       </c>
       <c r="C344" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.2">
@@ -5792,7 +5795,7 @@
         <v>90</v>
       </c>
       <c r="C345" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.2">
@@ -5803,7 +5806,7 @@
         <v>90</v>
       </c>
       <c r="C346" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.2">
@@ -5814,7 +5817,7 @@
         <v>241</v>
       </c>
       <c r="C347" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.2">
@@ -5825,7 +5828,7 @@
         <v>11</v>
       </c>
       <c r="C348" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.2">
@@ -5836,7 +5839,7 @@
         <v>198</v>
       </c>
       <c r="C349" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.2">
@@ -5847,7 +5850,7 @@
         <v>29</v>
       </c>
       <c r="C350" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
@@ -5858,7 +5861,7 @@
         <v>11</v>
       </c>
       <c r="C351" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
@@ -5869,7 +5872,7 @@
         <v>154</v>
       </c>
       <c r="C352" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
@@ -5880,7 +5883,7 @@
         <v>198</v>
       </c>
       <c r="C353" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
@@ -5891,7 +5894,7 @@
         <v>6</v>
       </c>
       <c r="C354" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.2">
@@ -5902,7 +5905,7 @@
         <v>11</v>
       </c>
       <c r="C355" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.2">
@@ -5913,7 +5916,7 @@
         <v>44</v>
       </c>
       <c r="C356" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.2">
@@ -5924,7 +5927,7 @@
         <v>36</v>
       </c>
       <c r="C357" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.2">
@@ -5935,7 +5938,7 @@
         <v>29</v>
       </c>
       <c r="C358" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.2">
@@ -5946,7 +5949,7 @@
         <v>8</v>
       </c>
       <c r="C359" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.2">
@@ -5957,7 +5960,7 @@
         <v>90</v>
       </c>
       <c r="C360" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.2">
@@ -5968,7 +5971,7 @@
         <v>61</v>
       </c>
       <c r="C361" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.2">
@@ -5979,7 +5982,7 @@
         <v>6</v>
       </c>
       <c r="C362" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.2">
@@ -5990,7 +5993,7 @@
         <v>90</v>
       </c>
       <c r="C363" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.2">
@@ -6001,7 +6004,7 @@
         <v>61</v>
       </c>
       <c r="C364" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.2">
@@ -6012,7 +6015,7 @@
         <v>59</v>
       </c>
       <c r="C365" t="s">
-        <v>396</v>
+        <v>526</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.2">
@@ -6023,7 +6026,7 @@
         <v>6</v>
       </c>
       <c r="C366" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.2">
@@ -6034,7 +6037,7 @@
         <v>11</v>
       </c>
       <c r="C367" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.2">
@@ -6042,10 +6045,10 @@
         <v>367</v>
       </c>
       <c r="B368" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C368" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.2">
@@ -6056,7 +6059,7 @@
         <v>6</v>
       </c>
       <c r="C369" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.2">
@@ -6067,7 +6070,7 @@
         <v>59</v>
       </c>
       <c r="C370" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.2">
@@ -6078,7 +6081,7 @@
         <v>18</v>
       </c>
       <c r="C371" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
@@ -6089,7 +6092,7 @@
         <v>241</v>
       </c>
       <c r="C372" t="s">
-        <v>404</v>
+        <v>527</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
@@ -6100,7 +6103,7 @@
         <v>198</v>
       </c>
       <c r="C373" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.2">
@@ -6111,7 +6114,7 @@
         <v>68</v>
       </c>
       <c r="C374" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
@@ -6122,7 +6125,7 @@
         <v>44</v>
       </c>
       <c r="C375" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.2">
@@ -6133,7 +6136,7 @@
         <v>11</v>
       </c>
       <c r="C376" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.2">
@@ -6144,7 +6147,7 @@
         <v>11</v>
       </c>
       <c r="C377" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.2">
@@ -6155,7 +6158,7 @@
         <v>132</v>
       </c>
       <c r="C378" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.2">
@@ -6166,7 +6169,7 @@
         <v>44</v>
       </c>
       <c r="C379" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.2">
@@ -6177,7 +6180,7 @@
         <v>36</v>
       </c>
       <c r="C380" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.2">
@@ -6188,7 +6191,7 @@
         <v>11</v>
       </c>
       <c r="C381" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.2">
@@ -6199,7 +6202,7 @@
         <v>241</v>
       </c>
       <c r="C382" t="s">
-        <v>414</v>
+        <v>528</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.2">
@@ -6210,7 +6213,7 @@
         <v>11</v>
       </c>
       <c r="C383" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.2">
@@ -6221,7 +6224,7 @@
         <v>29</v>
       </c>
       <c r="C384" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.2">
@@ -6232,7 +6235,7 @@
         <v>29</v>
       </c>
       <c r="C385" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.2">
@@ -6243,7 +6246,7 @@
         <v>90</v>
       </c>
       <c r="C386" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.2">
@@ -6254,7 +6257,7 @@
         <v>3</v>
       </c>
       <c r="C387" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.2">
@@ -6265,7 +6268,7 @@
         <v>90</v>
       </c>
       <c r="C388" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.2">
@@ -6276,7 +6279,7 @@
         <v>36</v>
       </c>
       <c r="C389" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.2">
@@ -6287,7 +6290,7 @@
         <v>154</v>
       </c>
       <c r="C390" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.2">
@@ -6298,7 +6301,7 @@
         <v>61</v>
       </c>
       <c r="C391" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.2">
@@ -6309,7 +6312,7 @@
         <v>29</v>
       </c>
       <c r="C392" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.2">
@@ -6320,7 +6323,7 @@
         <v>36</v>
       </c>
       <c r="C393" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.2">
@@ -6328,10 +6331,10 @@
         <v>393</v>
       </c>
       <c r="B394" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="C394" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.2">
@@ -6342,7 +6345,7 @@
         <v>44</v>
       </c>
       <c r="C395" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.2">
@@ -6353,7 +6356,7 @@
         <v>44</v>
       </c>
       <c r="C396" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.2">
@@ -6364,7 +6367,7 @@
         <v>44</v>
       </c>
       <c r="C397" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.2">
@@ -6375,7 +6378,7 @@
         <v>36</v>
       </c>
       <c r="C398" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.2">
@@ -6386,7 +6389,7 @@
         <v>198</v>
       </c>
       <c r="C399" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.2">
@@ -6397,7 +6400,7 @@
         <v>241</v>
       </c>
       <c r="C400" t="s">
-        <v>433</v>
+        <v>529</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.2">
@@ -6408,7 +6411,7 @@
         <v>198</v>
       </c>
       <c r="C401" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.2">
@@ -6419,7 +6422,7 @@
         <v>11</v>
       </c>
       <c r="C402" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.2">
@@ -6430,7 +6433,7 @@
         <v>44</v>
       </c>
       <c r="C403" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.2">
@@ -6438,10 +6441,10 @@
         <v>403</v>
       </c>
       <c r="B404" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C404" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.2">
@@ -6452,7 +6455,7 @@
         <v>44</v>
       </c>
       <c r="C405" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.2">
@@ -6463,7 +6466,7 @@
         <v>11</v>
       </c>
       <c r="C406" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.2">
@@ -6474,7 +6477,7 @@
         <v>36</v>
       </c>
       <c r="C407" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.2">
@@ -6485,7 +6488,7 @@
         <v>11</v>
       </c>
       <c r="C408" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.2">
@@ -6496,7 +6499,7 @@
         <v>90</v>
       </c>
       <c r="C409" t="s">
-        <v>442</v>
+        <v>535</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.2">
@@ -6507,7 +6510,7 @@
         <v>36</v>
       </c>
       <c r="C410" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.2">
@@ -6518,7 +6521,7 @@
         <v>36</v>
       </c>
       <c r="C411" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.2">
@@ -6529,7 +6532,7 @@
         <v>11</v>
       </c>
       <c r="C412" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.2">
@@ -6537,10 +6540,10 @@
         <v>412</v>
       </c>
       <c r="B413" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C413" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.2">
@@ -6551,7 +6554,7 @@
         <v>6</v>
       </c>
       <c r="C414" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.2">
@@ -6562,7 +6565,7 @@
         <v>61</v>
       </c>
       <c r="C415" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.2">
@@ -6573,7 +6576,7 @@
         <v>198</v>
       </c>
       <c r="C416" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.2">
@@ -6584,7 +6587,7 @@
         <v>36</v>
       </c>
       <c r="C417" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.2">
@@ -6595,7 +6598,7 @@
         <v>6</v>
       </c>
       <c r="C418" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.2">
@@ -6606,7 +6609,7 @@
         <v>3</v>
       </c>
       <c r="C419" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.2">
@@ -6617,7 +6620,7 @@
         <v>18</v>
       </c>
       <c r="C420" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.2">
@@ -6628,7 +6631,7 @@
         <v>6</v>
       </c>
       <c r="C421" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.2">
@@ -6639,7 +6642,7 @@
         <v>90</v>
       </c>
       <c r="C422" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.2">
@@ -6650,7 +6653,7 @@
         <v>11</v>
       </c>
       <c r="C423" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.2">
@@ -6661,7 +6664,7 @@
         <v>6</v>
       </c>
       <c r="C424" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.2">
@@ -6672,7 +6675,7 @@
         <v>29</v>
       </c>
       <c r="C425" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.2">
@@ -6683,7 +6686,7 @@
         <v>198</v>
       </c>
       <c r="C426" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.2">
@@ -6694,7 +6697,7 @@
         <v>44</v>
       </c>
       <c r="C427" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.2">
@@ -6705,7 +6708,7 @@
         <v>11</v>
       </c>
       <c r="C428" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.2">
@@ -6716,7 +6719,7 @@
         <v>150</v>
       </c>
       <c r="C429" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.2">
@@ -6727,7 +6730,7 @@
         <v>44</v>
       </c>
       <c r="C430" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.2">
@@ -6735,10 +6738,10 @@
         <v>430</v>
       </c>
       <c r="B431" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C431" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.2">
@@ -6749,7 +6752,7 @@
         <v>36</v>
       </c>
       <c r="C432" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.2">
@@ -6760,7 +6763,7 @@
         <v>6</v>
       </c>
       <c r="C433" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.2">
@@ -6771,7 +6774,7 @@
         <v>36</v>
       </c>
       <c r="C434" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.2">
@@ -6782,7 +6785,7 @@
         <v>44</v>
       </c>
       <c r="C435" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.2">
@@ -6793,7 +6796,7 @@
         <v>36</v>
       </c>
       <c r="C436" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.2">
@@ -6804,7 +6807,7 @@
         <v>90</v>
       </c>
       <c r="C437" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.2">
@@ -6815,7 +6818,7 @@
         <v>6</v>
       </c>
       <c r="C438" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.2">
@@ -6826,7 +6829,7 @@
         <v>29</v>
       </c>
       <c r="C439" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.2">
@@ -6837,7 +6840,7 @@
         <v>29</v>
       </c>
       <c r="C440" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.2">
@@ -6848,7 +6851,7 @@
         <v>90</v>
       </c>
       <c r="C441" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.2">
@@ -6856,10 +6859,10 @@
         <v>441</v>
       </c>
       <c r="B442" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C442" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.2">
@@ -6870,7 +6873,7 @@
         <v>6</v>
       </c>
       <c r="C443" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.2">
@@ -6881,7 +6884,7 @@
         <v>177</v>
       </c>
       <c r="C444" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.2">
@@ -6889,10 +6892,10 @@
         <v>444</v>
       </c>
       <c r="B445" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="C445" t="s">
-        <v>480</v>
+        <v>530</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.2">
@@ -6903,7 +6906,7 @@
         <v>18</v>
       </c>
       <c r="C446" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.2">
@@ -6911,10 +6914,10 @@
         <v>446</v>
       </c>
       <c r="B447" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C447" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.2">
@@ -6925,7 +6928,7 @@
         <v>44</v>
       </c>
       <c r="C448" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.2">
@@ -6936,7 +6939,7 @@
         <v>29</v>
       </c>
       <c r="C449" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.2">
@@ -6947,7 +6950,7 @@
         <v>44</v>
       </c>
       <c r="C450" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.2">
@@ -6958,7 +6961,7 @@
         <v>198</v>
       </c>
       <c r="C451" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.2">
@@ -6969,7 +6972,7 @@
         <v>44</v>
       </c>
       <c r="C452" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.2">
@@ -6980,7 +6983,7 @@
         <v>68</v>
       </c>
       <c r="C453" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.2">
@@ -6991,7 +6994,7 @@
         <v>198</v>
       </c>
       <c r="C454" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.2">
@@ -6999,10 +7002,10 @@
         <v>454</v>
       </c>
       <c r="B455" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="C455" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.2">
@@ -7013,7 +7016,7 @@
         <v>36</v>
       </c>
       <c r="C456" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.2">
@@ -7024,7 +7027,7 @@
         <v>6</v>
       </c>
       <c r="C457" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.2">
@@ -7035,7 +7038,7 @@
         <v>36</v>
       </c>
       <c r="C458" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.2">
@@ -7046,7 +7049,7 @@
         <v>6</v>
       </c>
       <c r="C459" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.2">
@@ -7057,7 +7060,7 @@
         <v>6</v>
       </c>
       <c r="C460" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.2">
@@ -7068,7 +7071,7 @@
         <v>44</v>
       </c>
       <c r="C461" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.2">
@@ -7079,7 +7082,7 @@
         <v>29</v>
       </c>
       <c r="C462" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.2">
@@ -7090,7 +7093,7 @@
         <v>90</v>
       </c>
       <c r="C463" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.2">
@@ -7101,7 +7104,7 @@
         <v>59</v>
       </c>
       <c r="C464" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.2">
@@ -7112,7 +7115,7 @@
         <v>6</v>
       </c>
       <c r="C465" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.2">
@@ -7123,7 +7126,7 @@
         <v>198</v>
       </c>
       <c r="C466" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.2">
@@ -7134,7 +7137,7 @@
         <v>90</v>
       </c>
       <c r="C467" t="s">
-        <v>502</v>
+        <v>531</v>
       </c>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.2">
@@ -7145,7 +7148,7 @@
         <v>241</v>
       </c>
       <c r="C468" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.2">
@@ -7156,7 +7159,7 @@
         <v>11</v>
       </c>
       <c r="C469" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.2">
@@ -7167,7 +7170,7 @@
         <v>6</v>
       </c>
       <c r="C470" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.2">
@@ -7178,7 +7181,7 @@
         <v>29</v>
       </c>
       <c r="C471" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.2">
@@ -7189,7 +7192,7 @@
         <v>29</v>
       </c>
       <c r="C472" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.2">
@@ -7200,7 +7203,7 @@
         <v>167</v>
       </c>
       <c r="C473" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.2">
@@ -7211,7 +7214,7 @@
         <v>132</v>
       </c>
       <c r="C474" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.2">
@@ -7222,7 +7225,7 @@
         <v>241</v>
       </c>
       <c r="C475" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.2">
@@ -7233,7 +7236,7 @@
         <v>44</v>
       </c>
       <c r="C476" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.2">
@@ -7241,10 +7244,10 @@
         <v>476</v>
       </c>
       <c r="B477" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C477" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.2">
@@ -7255,7 +7258,7 @@
         <v>132</v>
       </c>
       <c r="C478" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.2">
@@ -7266,7 +7269,7 @@
         <v>3</v>
       </c>
       <c r="C479" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.2">
@@ -7277,7 +7280,7 @@
         <v>6</v>
       </c>
       <c r="C480" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.2">
@@ -7285,10 +7288,10 @@
         <v>480</v>
       </c>
       <c r="B481" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="C481" t="s">
-        <v>516</v>
+        <v>532</v>
       </c>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.2">
@@ -7299,7 +7302,7 @@
         <v>3</v>
       </c>
       <c r="C482" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.2">
@@ -7310,7 +7313,7 @@
         <v>90</v>
       </c>
       <c r="C483" t="s">
-        <v>518</v>
+        <v>534</v>
       </c>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.2">
@@ -7321,7 +7324,7 @@
         <v>154</v>
       </c>
       <c r="C484" t="s">
-        <v>519</v>
+        <v>508</v>
       </c>
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.2">
@@ -7332,7 +7335,7 @@
         <v>59</v>
       </c>
       <c r="C485" t="s">
-        <v>520</v>
+        <v>533</v>
       </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.2">
@@ -7343,7 +7346,7 @@
         <v>8</v>
       </c>
       <c r="C486" t="s">
-        <v>521</v>
+        <v>509</v>
       </c>
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.2">
@@ -7354,7 +7357,7 @@
         <v>103</v>
       </c>
       <c r="C487" t="s">
-        <v>522</v>
+        <v>510</v>
       </c>
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.2">
@@ -7362,10 +7365,10 @@
         <v>487</v>
       </c>
       <c r="B488" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C488" t="s">
-        <v>523</v>
+        <v>511</v>
       </c>
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.2">
@@ -7376,7 +7379,7 @@
         <v>44</v>
       </c>
       <c r="C489" t="s">
-        <v>524</v>
+        <v>512</v>
       </c>
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.2">
@@ -7387,7 +7390,7 @@
         <v>36</v>
       </c>
       <c r="C490" t="s">
-        <v>525</v>
+        <v>513</v>
       </c>
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.2">
@@ -7398,7 +7401,7 @@
         <v>150</v>
       </c>
       <c r="C491" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.2">
@@ -7409,7 +7412,7 @@
         <v>90</v>
       </c>
       <c r="C492" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.2">
@@ -7420,7 +7423,7 @@
         <v>198</v>
       </c>
       <c r="C493" t="s">
-        <v>527</v>
+        <v>515</v>
       </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.2">
@@ -7431,7 +7434,7 @@
         <v>198</v>
       </c>
       <c r="C494" t="s">
-        <v>528</v>
+        <v>516</v>
       </c>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.2">
@@ -7442,7 +7445,7 @@
         <v>29</v>
       </c>
       <c r="C495" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.2">
@@ -7453,7 +7456,7 @@
         <v>6</v>
       </c>
       <c r="C496" t="s">
-        <v>530</v>
+        <v>518</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.2">
@@ -7464,7 +7467,7 @@
         <v>6</v>
       </c>
       <c r="C497" t="s">
-        <v>531</v>
+        <v>519</v>
       </c>
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.2">
@@ -7475,7 +7478,7 @@
         <v>36</v>
       </c>
       <c r="C498" t="s">
-        <v>532</v>
+        <v>520</v>
       </c>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.2">
@@ -7486,7 +7489,7 @@
         <v>132</v>
       </c>
       <c r="C499" t="s">
-        <v>533</v>
+        <v>521</v>
       </c>
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.2">
@@ -7497,7 +7500,7 @@
         <v>36</v>
       </c>
       <c r="C500" t="s">
-        <v>534</v>
+        <v>522</v>
       </c>
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.2">
@@ -7508,10 +7511,11 @@
         <v>44</v>
       </c>
       <c r="C501" t="s">
-        <v>535</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C501" xr:uid="{342C9819-C779-7E4D-BFB7-E36C0F9285F9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>